<commit_message>
merubah ketika login langsung masuk ke dashboard
</commit_message>
<xml_diff>
--- a/public/AsetData/importAset.xlsx
+++ b/public/AsetData/importAset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C405C57F-2B78-492E-B610-ACCF74368450}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0B5888-3371-44DD-A1BD-14800408379F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{9CBE1E65-8C51-4723-9D96-C31BA13FF0F9}"/>
   </bookViews>
@@ -199,7 +199,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,31 +211,16 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
+      <scheme val="major"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="3">
@@ -279,31 +264,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -623,36 +599,36 @@
   <dimension ref="A1:H999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="40.28515625" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="12.5703125" style="5"/>
+    <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="40.28515625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="12.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="2">
         <v>1</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -661,24 +637,24 @@
       <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>1</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -687,24 +663,24 @@
       <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>10</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -713,24 +689,24 @@
       <c r="G3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>5</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -739,24 +715,24 @@
       <c r="G4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -765,24 +741,24 @@
       <c r="G5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="2">
         <v>2</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -791,163 +767,163 @@
       <c r="G6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="2">
         <v>12</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="2">
         <v>2</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="2">
         <v>6</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="2">
         <v>20</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="2">
         <v>4</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="2">
         <v>1</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="2" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1940,5 +1916,6 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>